<commit_message>
rerun with new data sources & HMD switch
</commit_message>
<xml_diff>
--- a/data-raw/BfS/px-x-0102020000_104_AGE.xlsx
+++ b/data-raw/BfS/px-x-0102020000_104_AGE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <x:si>
     <x:t>Demographic balance by age and canton</x:t>
   </x:si>
@@ -335,6 +335,9 @@
   </x:si>
   <x:si>
     <x:t>99 years or older</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No indication</x:t>
   </x:si>
   <x:si>
     <x:t>&lt;B&gt;Meta information:&lt;/B&gt;
@@ -814,7 +817,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H143"/>
+  <x:dimension ref="A1:H144"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -1958,9 +1961,15 @@
         <x:v>3070</x:v>
       </x:c>
     </x:row>
-    <x:row r="105" spans="1:8">
-      <x:c r="A105" s="4" t="s">
+    <x:row r="104" spans="1:8">
+      <x:c r="F104" s="2" t="s">
         <x:v>107</x:v>
+      </x:c>
+      <x:c r="G104" s="3" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H104" s="3" t="n">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="106" spans="1:8">
@@ -2013,8 +2022,8 @@
         <x:v>117</x:v>
       </x:c>
     </x:row>
-    <x:row r="117" spans="1:8">
-      <x:c r="A117" s="0" t="s">
+    <x:row r="116" spans="1:8">
+      <x:c r="A116" s="4" t="s">
         <x:v>118</x:v>
       </x:c>
     </x:row>
@@ -2023,8 +2032,8 @@
         <x:v>119</x:v>
       </x:c>
     </x:row>
-    <x:row r="120" spans="1:8">
-      <x:c r="A120" s="0" t="s">
+    <x:row r="119" spans="1:8">
+      <x:c r="A119" s="0" t="s">
         <x:v>120</x:v>
       </x:c>
     </x:row>
@@ -2033,8 +2042,8 @@
         <x:v>121</x:v>
       </x:c>
     </x:row>
-    <x:row r="123" spans="1:8">
-      <x:c r="A123" s="0" t="s">
+    <x:row r="122" spans="1:8">
+      <x:c r="A122" s="0" t="s">
         <x:v>122</x:v>
       </x:c>
     </x:row>
@@ -2043,8 +2052,8 @@
         <x:v>123</x:v>
       </x:c>
     </x:row>
-    <x:row r="127" spans="1:8">
-      <x:c r="A127" s="0" t="s">
+    <x:row r="125" spans="1:8">
+      <x:c r="A125" s="0" t="s">
         <x:v>124</x:v>
       </x:c>
     </x:row>
@@ -2053,8 +2062,8 @@
         <x:v>125</x:v>
       </x:c>
     </x:row>
-    <x:row r="131" spans="1:8">
-      <x:c r="A131" s="0" t="s">
+    <x:row r="129" spans="1:8">
+      <x:c r="A129" s="0" t="s">
         <x:v>126</x:v>
       </x:c>
     </x:row>
@@ -2063,8 +2072,8 @@
         <x:v>127</x:v>
       </x:c>
     </x:row>
-    <x:row r="139" spans="1:8">
-      <x:c r="A139" s="0" t="s">
+    <x:row r="133" spans="1:8">
+      <x:c r="A133" s="0" t="s">
         <x:v>128</x:v>
       </x:c>
     </x:row>
@@ -2073,14 +2082,19 @@
         <x:v>129</x:v>
       </x:c>
     </x:row>
-    <x:row r="142" spans="1:8">
-      <x:c r="A142" s="0" t="s">
+    <x:row r="141" spans="1:8">
+      <x:c r="A141" s="0" t="s">
         <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="143" spans="1:8">
       <x:c r="A143" s="0" t="s">
         <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144" spans="1:8">
+      <x:c r="A144" s="0" t="s">
+        <x:v>132</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>